<commit_message>
added char and blob as possible data types on the Modify Dataset tab
</commit_message>
<xml_diff>
--- a/pages/images/Dataset_Model_Current_TEMPLATE.xlsx
+++ b/pages/images/Dataset_Model_Current_TEMPLATE.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Projects\DA_Operations\templates\dataset_logfile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MDWILKIE\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53592E4B-D075-443A-A9EE-BE81AC6EC3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF32037C-C215-49CD-8802-FF601974F541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="694" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="694" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset Model-New Dataset" sheetId="5" r:id="rId1"/>
     <sheet name="Dataset Model-Modify Dataset" sheetId="15" r:id="rId2"/>
-    <sheet name="Drop Downs" sheetId="4" state="hidden" r:id="rId3"/>
+    <sheet name="Drop Downs" sheetId="4" r:id="rId3"/>
     <sheet name="abbreviations" sheetId="13" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
@@ -4893,12 +4893,132 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="30" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="30" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="30" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="30" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="30" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="30" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -4908,11 +5028,41 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4920,132 +5070,6 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="30" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="30" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="30" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="30" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="30" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="30" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -5065,30 +5089,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5096,7 +5096,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="10">
     <dxf>
       <font>
         <b/>
@@ -5105,31 +5105,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5151,11 +5127,6 @@
         <i val="0"/>
         <color rgb="FFFF0000"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -5182,20 +5153,11 @@
         <i val="0"/>
         <color rgb="FFFF0000"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -5212,7 +5174,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5222,11 +5184,13 @@
         <i val="0"/>
         <color rgb="FFFF0000"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -6219,27 +6183,27 @@
   </sheetPr>
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.9" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="35.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="17.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.1796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="35.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.26953125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="27.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.54296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="35.5234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5234375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.47265625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="17.5234375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.15625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="35.5234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.26171875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="27.15625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.5234375" style="1" customWidth="1"/>
     <col min="11" max="11" width="16" style="1" customWidth="1"/>
     <col min="12" max="12" width="47" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="1"/>
+    <col min="13" max="16384" width="9.15625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="39" t="s">
         <v>281</v>
       </c>
@@ -6247,12 +6211,12 @@
         <v>289</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="5" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" s="5" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="36" t="s">
         <v>248</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="77"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="80"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -6263,7 +6227,7 @@
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
     </row>
-    <row r="3" spans="1:12" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -6277,93 +6241,93 @@
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="1:12" s="5" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" s="5" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="34" t="s">
         <v>264</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="89"/>
+      <c r="B4" s="90"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="92"/>
       <c r="F4" s="7"/>
       <c r="G4" s="35" t="s">
         <v>284</v>
       </c>
-      <c r="H4" s="68"/>
-      <c r="I4" s="69"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="104"/>
       <c r="K4" s="60" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="5" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="79" t="s">
+    <row r="5" spans="1:12" s="5" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A5" s="82" t="s">
         <v>265</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="83"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="86"/>
       <c r="F5" s="7"/>
       <c r="G5" s="35" t="s">
         <v>266</v>
       </c>
-      <c r="H5" s="68"/>
-      <c r="I5" s="69"/>
+      <c r="H5" s="103"/>
+      <c r="I5" s="104"/>
       <c r="K5" s="61" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="5" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="80"/>
-      <c r="B6" s="84"/>
-      <c r="C6" s="85"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="86"/>
+    <row r="6" spans="1:12" s="5" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="83"/>
+      <c r="B6" s="87"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="89"/>
       <c r="F6" s="7"/>
       <c r="G6" s="35" t="s">
         <v>267</v>
       </c>
-      <c r="H6" s="68"/>
-      <c r="I6" s="69"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="104"/>
       <c r="K6" s="61" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="5" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="98" t="s">
+    <row r="7" spans="1:12" s="5" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A7" s="101" t="s">
         <v>280</v>
       </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="83"/>
+      <c r="B7" s="84"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="86"/>
       <c r="F7" s="7"/>
       <c r="G7" s="35" t="s">
         <v>268</v>
       </c>
-      <c r="H7" s="68"/>
-      <c r="I7" s="69"/>
+      <c r="H7" s="103"/>
+      <c r="I7" s="104"/>
       <c r="K7" s="62" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="5" customFormat="1" ht="41.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="99"/>
-      <c r="B8" s="84"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="86"/>
+    <row r="8" spans="1:12" s="5" customFormat="1" ht="41.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A8" s="102"/>
+      <c r="B8" s="87"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="89"/>
       <c r="F8" s="7"/>
       <c r="G8" s="35" t="s">
         <v>273</v>
       </c>
-      <c r="H8" s="68"/>
-      <c r="I8" s="69"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="104"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
     </row>
-    <row r="9" spans="1:12" s="5" customFormat="1" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" s="5" customFormat="1" ht="41.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="41"/>
       <c r="B9" s="29"/>
       <c r="C9" s="29"/>
@@ -6377,7 +6341,7 @@
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
     </row>
-    <row r="10" spans="1:12" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -6391,17 +6355,17 @@
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
     </row>
-    <row r="11" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="90" t="s">
+    <row r="11" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="91"/>
-      <c r="C11" s="92"/>
-      <c r="D11" s="96" t="s">
+      <c r="B11" s="94"/>
+      <c r="C11" s="95"/>
+      <c r="D11" s="99" t="s">
         <v>259</v>
       </c>
-      <c r="E11" s="91"/>
-      <c r="F11" s="92"/>
+      <c r="E11" s="94"/>
+      <c r="F11" s="95"/>
       <c r="G11" s="46" t="s">
         <v>227</v>
       </c>
@@ -6411,13 +6375,13 @@
       <c r="K11" s="50"/>
       <c r="L11" s="11"/>
     </row>
-    <row r="12" spans="1:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="93"/>
-      <c r="B12" s="94"/>
-      <c r="C12" s="95"/>
-      <c r="D12" s="97"/>
-      <c r="E12" s="94"/>
-      <c r="F12" s="95"/>
+    <row r="12" spans="1:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="96"/>
+      <c r="B12" s="97"/>
+      <c r="C12" s="98"/>
+      <c r="D12" s="100"/>
+      <c r="E12" s="97"/>
+      <c r="F12" s="98"/>
       <c r="G12" s="45"/>
       <c r="H12" s="11"/>
       <c r="I12" s="12"/>
@@ -6425,39 +6389,39 @@
       <c r="K12" s="49"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="J13" s="49"/>
       <c r="K13" s="49"/>
     </row>
-    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="J14" s="20"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="111" t="s">
+    <row r="15" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="76" t="s">
         <v>241</v>
       </c>
-      <c r="B15" s="112"/>
-      <c r="C15" s="113"/>
-      <c r="D15" s="65" t="s">
+      <c r="B15" s="77"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="105" t="s">
         <v>243</v>
       </c>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="67"/>
+      <c r="E15" s="106"/>
+      <c r="F15" s="106"/>
+      <c r="G15" s="106"/>
+      <c r="H15" s="107"/>
       <c r="I15" s="57" t="s">
         <v>240</v>
       </c>
-      <c r="J15" s="107" t="s">
+      <c r="J15" s="72" t="s">
         <v>242</v>
       </c>
-      <c r="K15" s="107"/>
+      <c r="K15" s="72"/>
       <c r="L15" s="48" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="71.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" s="16" t="s">
         <v>6</v>
       </c>
@@ -6485,15 +6449,15 @@
       <c r="I16" s="59" t="s">
         <v>251</v>
       </c>
-      <c r="J16" s="78" t="s">
+      <c r="J16" s="81" t="s">
         <v>245</v>
       </c>
-      <c r="K16" s="78"/>
+      <c r="K16" s="81"/>
       <c r="L16" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="13"/>
@@ -6516,13 +6480,13 @@
       <c r="I17" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="J17" s="108" t="s">
+      <c r="J17" s="73" t="s">
         <v>232</v>
       </c>
-      <c r="K17" s="108"/>
+      <c r="K17" s="73"/>
       <c r="L17" s="40"/>
     </row>
-    <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A18" s="13"/>
       <c r="B18" s="14"/>
       <c r="C18" s="13"/>
@@ -6537,11 +6501,11 @@
         <f>VLOOKUP($D18,abbreviations!$A$1:$B$99999,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J18" s="63"/>
-      <c r="K18" s="64"/>
+      <c r="J18" s="70"/>
+      <c r="K18" s="71"/>
       <c r="L18" s="21"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A19" s="13"/>
       <c r="B19" s="14"/>
       <c r="C19" s="13"/>
@@ -6554,11 +6518,11 @@
         <f>VLOOKUP($D19,abbreviations!$A$1:$B$99999,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J19" s="63"/>
-      <c r="K19" s="64"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="71"/>
       <c r="L19" s="21"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A20" s="13"/>
       <c r="B20" s="14"/>
       <c r="C20" s="13"/>
@@ -6571,11 +6535,11 @@
         <f>VLOOKUP($D20,abbreviations!$A$1:$B$99999,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J20" s="63"/>
-      <c r="K20" s="64"/>
+      <c r="J20" s="70"/>
+      <c r="K20" s="71"/>
       <c r="L20" s="21"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A21" s="13"/>
       <c r="B21" s="14"/>
       <c r="C21" s="13"/>
@@ -6588,11 +6552,11 @@
         <f>VLOOKUP($D21,abbreviations!$A$1:$B$99999,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J21" s="63"/>
-      <c r="K21" s="64"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="71"/>
       <c r="L21" s="21"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A22" s="13"/>
       <c r="B22" s="14"/>
       <c r="C22" s="13"/>
@@ -6605,11 +6569,11 @@
         <f>VLOOKUP($D22,abbreviations!$A$1:$B$99999,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J22" s="63"/>
-      <c r="K22" s="64"/>
+      <c r="J22" s="70"/>
+      <c r="K22" s="71"/>
       <c r="L22" s="21"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A23" s="13"/>
       <c r="B23" s="14"/>
       <c r="C23" s="13"/>
@@ -6622,11 +6586,11 @@
         <f>VLOOKUP($D23,abbreviations!$A$1:$B$99999,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J23" s="63"/>
-      <c r="K23" s="64"/>
+      <c r="J23" s="70"/>
+      <c r="K23" s="71"/>
       <c r="L23" s="21"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A24" s="13"/>
       <c r="B24" s="14"/>
       <c r="C24" s="13"/>
@@ -6639,11 +6603,11 @@
         <f>VLOOKUP($D24,abbreviations!$A$1:$B$99999,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J24" s="63"/>
-      <c r="K24" s="64"/>
+      <c r="J24" s="70"/>
+      <c r="K24" s="71"/>
       <c r="L24" s="21"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
       <c r="C25" s="13"/>
@@ -6656,11 +6620,11 @@
         <f>VLOOKUP($D25,abbreviations!$A$1:$B$99999,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J25" s="63"/>
-      <c r="K25" s="64"/>
+      <c r="J25" s="70"/>
+      <c r="K25" s="71"/>
       <c r="L25" s="21"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A26" s="13"/>
       <c r="B26" s="14"/>
       <c r="C26" s="13"/>
@@ -6673,11 +6637,11 @@
         <f>VLOOKUP($D26,abbreviations!$A$1:$B$99999,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J26" s="63"/>
-      <c r="K26" s="64"/>
+      <c r="J26" s="70"/>
+      <c r="K26" s="71"/>
       <c r="L26" s="21"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A27" s="13"/>
       <c r="B27" s="14"/>
       <c r="C27" s="13"/>
@@ -6690,11 +6654,11 @@
         <f>VLOOKUP($D27,abbreviations!$A$1:$B$99999,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J27" s="63"/>
-      <c r="K27" s="64"/>
+      <c r="J27" s="70"/>
+      <c r="K27" s="71"/>
       <c r="L27" s="21"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A28" s="13"/>
       <c r="B28" s="14"/>
       <c r="C28" s="13"/>
@@ -6707,11 +6671,11 @@
         <f>VLOOKUP($D28,abbreviations!$A$1:$B$99999,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J28" s="63"/>
-      <c r="K28" s="64"/>
+      <c r="J28" s="70"/>
+      <c r="K28" s="71"/>
       <c r="L28" s="21"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A29" s="13"/>
       <c r="B29" s="14"/>
       <c r="C29" s="13"/>
@@ -6724,11 +6688,11 @@
         <f>VLOOKUP($D29,abbreviations!$A$1:$B$99999,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J29" s="63"/>
-      <c r="K29" s="64"/>
+      <c r="J29" s="70"/>
+      <c r="K29" s="71"/>
       <c r="L29" s="21"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A30" s="13"/>
       <c r="B30" s="14"/>
       <c r="C30" s="13"/>
@@ -6741,11 +6705,11 @@
         <f>VLOOKUP($D30,abbreviations!$A$1:$B$99999,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J30" s="63"/>
-      <c r="K30" s="64"/>
+      <c r="J30" s="70"/>
+      <c r="K30" s="71"/>
       <c r="L30" s="21"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A31" s="13"/>
       <c r="B31" s="14"/>
       <c r="C31" s="13"/>
@@ -6758,11 +6722,11 @@
         <f>VLOOKUP($D31,abbreviations!$A$1:$B$99999,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J31" s="63"/>
-      <c r="K31" s="64"/>
+      <c r="J31" s="70"/>
+      <c r="K31" s="71"/>
       <c r="L31" s="21"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A32" s="13"/>
       <c r="B32" s="14"/>
       <c r="C32" s="13"/>
@@ -6775,11 +6739,11 @@
         <f>VLOOKUP($D32,abbreviations!$A$1:$B$99999,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J32" s="63"/>
-      <c r="K32" s="64"/>
+      <c r="J32" s="70"/>
+      <c r="K32" s="71"/>
       <c r="L32" s="21"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A33" s="13"/>
       <c r="B33" s="14"/>
       <c r="C33" s="13"/>
@@ -6792,11 +6756,11 @@
         <f>VLOOKUP($D33,abbreviations!$A$1:$B$99999,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J33" s="63"/>
-      <c r="K33" s="64"/>
+      <c r="J33" s="70"/>
+      <c r="K33" s="71"/>
       <c r="L33" s="21"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A34" s="13"/>
       <c r="B34" s="14"/>
       <c r="C34" s="13"/>
@@ -6809,11 +6773,11 @@
         <f>VLOOKUP($D34,abbreviations!$A$1:$B$99999,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J34" s="63"/>
-      <c r="K34" s="64"/>
+      <c r="J34" s="70"/>
+      <c r="K34" s="71"/>
       <c r="L34" s="21"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A35" s="13"/>
       <c r="B35" s="14"/>
       <c r="C35" s="13"/>
@@ -6826,11 +6790,11 @@
         <f>VLOOKUP($D35,abbreviations!$A$1:$B$99999,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J35" s="63"/>
-      <c r="K35" s="64"/>
+      <c r="J35" s="70"/>
+      <c r="K35" s="71"/>
       <c r="L35" s="21"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A36" s="13"/>
       <c r="B36" s="14"/>
       <c r="C36" s="13"/>
@@ -6843,11 +6807,11 @@
         <f>VLOOKUP($D36,abbreviations!$A$1:$B$99999,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J36" s="63"/>
-      <c r="K36" s="64"/>
+      <c r="J36" s="70"/>
+      <c r="K36" s="71"/>
       <c r="L36" s="21"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A37" s="13"/>
       <c r="B37" s="14"/>
       <c r="C37" s="13"/>
@@ -6860,11 +6824,11 @@
         <f>VLOOKUP($D37,abbreviations!$A$1:$B$99999,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="J37" s="63"/>
-      <c r="K37" s="64"/>
+      <c r="J37" s="70"/>
+      <c r="K37" s="71"/>
       <c r="L37" s="21"/>
     </row>
-    <row r="38" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A38" s="13"/>
       <c r="B38" s="14"/>
       <c r="C38" s="13"/>
@@ -6884,18 +6848,18 @@
       <c r="I38" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="J38" s="109" t="s">
+      <c r="J38" s="74" t="s">
         <v>235</v>
       </c>
-      <c r="K38" s="110"/>
+      <c r="K38" s="75"/>
       <c r="L38" s="8"/>
     </row>
-    <row r="39" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="100" t="s">
+    <row r="39" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A39" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="101"/>
-      <c r="C39" s="102"/>
+      <c r="B39" s="64"/>
+      <c r="C39" s="65"/>
       <c r="D39" s="3" t="s">
         <v>61</v>
       </c>
@@ -6914,16 +6878,16 @@
       <c r="I39" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="J39" s="109" t="s">
+      <c r="J39" s="74" t="s">
         <v>233</v>
       </c>
-      <c r="K39" s="110"/>
+      <c r="K39" s="75"/>
       <c r="L39" s="8"/>
     </row>
-    <row r="40" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="103"/>
-      <c r="B40" s="104"/>
-      <c r="C40" s="105"/>
+    <row r="40" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A40" s="66"/>
+      <c r="B40" s="67"/>
+      <c r="C40" s="68"/>
       <c r="D40" s="3" t="s">
         <v>62</v>
       </c>
@@ -6942,16 +6906,16 @@
       <c r="I40" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="J40" s="109" t="s">
+      <c r="J40" s="74" t="s">
         <v>234</v>
       </c>
-      <c r="K40" s="110"/>
+      <c r="K40" s="75"/>
       <c r="L40" s="8"/>
     </row>
-    <row r="41" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="103"/>
-      <c r="B41" s="104"/>
-      <c r="C41" s="105"/>
+    <row r="41" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A41" s="66"/>
+      <c r="B41" s="67"/>
+      <c r="C41" s="68"/>
       <c r="D41" s="3" t="s">
         <v>7</v>
       </c>
@@ -6970,16 +6934,16 @@
       <c r="I41" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J41" s="109" t="s">
+      <c r="J41" s="74" t="s">
         <v>236</v>
       </c>
-      <c r="K41" s="110"/>
+      <c r="K41" s="75"/>
       <c r="L41" s="8"/>
     </row>
-    <row r="42" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="103"/>
-      <c r="B42" s="104"/>
-      <c r="C42" s="105"/>
+    <row r="42" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A42" s="66"/>
+      <c r="B42" s="67"/>
+      <c r="C42" s="68"/>
       <c r="D42" s="3" t="s">
         <v>64</v>
       </c>
@@ -6994,27 +6958,58 @@
       <c r="I42" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="J42" s="109" t="s">
+      <c r="J42" s="74" t="s">
         <v>237</v>
       </c>
-      <c r="K42" s="110"/>
+      <c r="K42" s="75"/>
       <c r="L42" s="8"/>
     </row>
-    <row r="44" spans="1:12" s="33" customFormat="1" ht="68.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="106" t="s">
+    <row r="44" spans="1:12" s="33" customFormat="1" ht="68.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A44" s="69" t="s">
         <v>262</v>
       </c>
-      <c r="B44" s="106"/>
-      <c r="C44" s="106"/>
-      <c r="D44" s="106"/>
-      <c r="E44" s="106"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B44" s="69"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="69"/>
+      <c r="E44" s="69"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A45" s="33"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="47">
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="D15:H15"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:E6"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:E8"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
     <mergeCell ref="A39:C42"/>
     <mergeCell ref="A44:E44"/>
     <mergeCell ref="J18:K18"/>
@@ -7031,61 +7026,30 @@
     <mergeCell ref="J26:K26"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="J21:K21"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:E6"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:E8"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="D15:H15"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="J28:K28"/>
   </mergeCells>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="expression" dxfId="9" priority="2">
+      <formula>LEN(A12) &gt;30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="expression" dxfId="8" priority="1">
+      <formula>LEN(D12) &gt;30</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D18:D38">
-    <cfRule type="expression" dxfId="12" priority="16">
+    <cfRule type="expression" dxfId="7" priority="16">
       <formula>LEN(D18)&gt;30</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I18:I38">
-    <cfRule type="expression" dxfId="11" priority="19">
-      <formula>LEN(I18)&gt;10</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>LEN(G12) &gt;30</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="9" priority="1">
-      <formula>LEN(D12) &gt;30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
-    <cfRule type="expression" dxfId="8" priority="2">
-      <formula>LEN(A12) &gt;30</formula>
+  <conditionalFormatting sqref="I18:I38">
+    <cfRule type="expression" dxfId="5" priority="19">
+      <formula>LEN(I18)&gt;10</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="81" yWindow="814" count="4">
@@ -7176,40 +7140,40 @@
   </sheetPr>
   <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.9" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="30.81640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1796875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="30.7890625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.15625" style="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5234375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.26953125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="41.1796875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.26953125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="34.1796875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="35.453125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.1796875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25.26171875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="41.15625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.26171875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="34.15625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="35.47265625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.15625" style="1" customWidth="1"/>
     <col min="15" max="15" width="28" style="1" customWidth="1"/>
-    <col min="16" max="16" width="8.26953125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10.81640625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="7.81640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="14.1796875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="13.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="2.26953125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="34.54296875" style="1" customWidth="1"/>
-    <col min="24" max="24" width="43.453125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="2.453125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="42.453125" style="1" customWidth="1"/>
-    <col min="27" max="16384" width="9.1796875" style="1"/>
+    <col min="16" max="16" width="8.26171875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="10.7890625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="7.7890625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="14.15625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="13.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.7890625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="2.26171875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="34.5234375" style="1" customWidth="1"/>
+    <col min="24" max="24" width="43.47265625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="2.47265625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="42.47265625" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.15625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="39" t="s">
         <v>282</v>
       </c>
@@ -7218,7 +7182,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="5" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" s="5" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="37" t="s">
         <v>248</v>
       </c>
@@ -7248,7 +7212,7 @@
       <c r="Y2" s="7"/>
       <c r="Z2" s="7"/>
     </row>
-    <row r="3" spans="1:26" s="5" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" s="5" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="52"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -7276,7 +7240,7 @@
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
     </row>
-    <row r="4" spans="1:26" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -7286,10 +7250,10 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
-      <c r="J4" s="70" t="s">
+      <c r="J4" s="120" t="s">
         <v>66</v>
       </c>
-      <c r="K4" s="71"/>
+      <c r="K4" s="121"/>
       <c r="L4" s="25"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
@@ -7306,22 +7270,22 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="118" t="s">
+    <row r="5" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="126" t="s">
         <v>253</v>
       </c>
-      <c r="B5" s="120"/>
-      <c r="C5" s="124" t="s">
+      <c r="B5" s="128"/>
+      <c r="C5" s="111" t="s">
         <v>260</v>
       </c>
-      <c r="D5" s="125"/>
+      <c r="D5" s="112"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
-      <c r="J5" s="72" t="s">
+      <c r="J5" s="118" t="s">
         <v>238</v>
       </c>
-      <c r="K5" s="73"/>
+      <c r="K5" s="119"/>
       <c r="L5" s="20"/>
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
@@ -7336,19 +7300,19 @@
       <c r="Y5" s="25"/>
       <c r="Z5" s="11"/>
     </row>
-    <row r="6" spans="1:26" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="114"/>
-      <c r="B6" s="115"/>
-      <c r="C6" s="126"/>
-      <c r="D6" s="127"/>
+    <row r="6" spans="1:26" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="122"/>
+      <c r="B6" s="123"/>
+      <c r="C6" s="113"/>
+      <c r="D6" s="114"/>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
       <c r="H6" s="28"/>
       <c r="I6" s="28"/>
-      <c r="J6" s="72" t="s">
+      <c r="J6" s="118" t="s">
         <v>239</v>
       </c>
-      <c r="K6" s="73"/>
+      <c r="K6" s="119"/>
       <c r="L6" s="20"/>
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
@@ -7363,51 +7327,51 @@
       <c r="Y6" s="20"/>
       <c r="Z6" s="12"/>
     </row>
-    <row r="7" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J7" s="74" t="s">
+    <row r="7" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J7" s="116" t="s">
         <v>285</v>
       </c>
-      <c r="K7" s="75"/>
+      <c r="K7" s="117"/>
       <c r="L7" s="20"/>
       <c r="Y7" s="20"/>
     </row>
-    <row r="8" spans="1:26" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="121" t="s">
+    <row r="8" spans="1:26" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A8" s="108" t="s">
         <v>290</v>
       </c>
-      <c r="B8" s="122"/>
-      <c r="C8" s="123"/>
-      <c r="D8" s="69"/>
+      <c r="B8" s="109"/>
+      <c r="C8" s="110"/>
+      <c r="D8" s="104"/>
       <c r="J8" s="20"/>
       <c r="K8" s="20"/>
       <c r="L8" s="20"/>
       <c r="Y8" s="20"/>
     </row>
-    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
       <c r="Y9" s="20"/>
     </row>
-    <row r="10" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="118" t="s">
+    <row r="10" spans="1:26" ht="13.2" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="11" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="126" t="s">
         <v>255</v>
       </c>
-      <c r="B11" s="119"/>
-      <c r="C11" s="119"/>
-      <c r="D11" s="119"/>
-      <c r="E11" s="119"/>
-      <c r="F11" s="119"/>
-      <c r="G11" s="119"/>
-      <c r="H11" s="120"/>
+      <c r="B11" s="127"/>
+      <c r="C11" s="127"/>
+      <c r="D11" s="127"/>
+      <c r="E11" s="127"/>
+      <c r="F11" s="127"/>
+      <c r="G11" s="127"/>
+      <c r="H11" s="128"/>
       <c r="I11" s="30" t="s">
         <v>261</v>
       </c>
-      <c r="J11" s="128" t="s">
+      <c r="J11" s="115" t="s">
         <v>254</v>
       </c>
-      <c r="K11" s="128"/>
+      <c r="K11" s="115"/>
       <c r="L11" s="47" t="s">
         <v>286</v>
       </c>
@@ -7415,7 +7379,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" ht="42" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" s="18" t="s">
         <v>252</v>
       </c>
@@ -7443,10 +7407,10 @@
       <c r="I12" s="17" t="s">
         <v>258</v>
       </c>
-      <c r="J12" s="78" t="s">
+      <c r="J12" s="81" t="s">
         <v>245</v>
       </c>
-      <c r="K12" s="78"/>
+      <c r="K12" s="81"/>
       <c r="L12" s="44" t="s">
         <v>287</v>
       </c>
@@ -7454,7 +7418,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.5">
       <c r="A13" s="23" t="s">
         <v>54</v>
       </c>
@@ -7466,12 +7430,12 @@
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
-      <c r="J13" s="63"/>
-      <c r="K13" s="64"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="71"/>
       <c r="L13" s="54"/>
       <c r="M13" s="26"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.5">
       <c r="A14" s="23"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -7481,12 +7445,12 @@
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
       <c r="I14" s="15"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="64"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="71"/>
       <c r="L14" s="54"/>
       <c r="M14" s="26"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.5">
       <c r="A15" s="23"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -7496,12 +7460,12 @@
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="64"/>
+      <c r="J15" s="70"/>
+      <c r="K15" s="71"/>
       <c r="L15" s="54"/>
       <c r="M15" s="26"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.5">
       <c r="A16" s="23"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
@@ -7511,12 +7475,12 @@
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
-      <c r="J16" s="63"/>
-      <c r="K16" s="64"/>
+      <c r="J16" s="70"/>
+      <c r="K16" s="71"/>
       <c r="L16" s="54"/>
       <c r="M16" s="26"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A17" s="23"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -7526,12 +7490,12 @@
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
       <c r="I17" s="15"/>
-      <c r="J17" s="63"/>
-      <c r="K17" s="64"/>
+      <c r="J17" s="70"/>
+      <c r="K17" s="71"/>
       <c r="L17" s="54"/>
       <c r="M17" s="26"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A18" s="23"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -7541,12 +7505,12 @@
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
-      <c r="J18" s="63"/>
-      <c r="K18" s="64"/>
+      <c r="J18" s="70"/>
+      <c r="K18" s="71"/>
       <c r="L18" s="54"/>
       <c r="M18" s="26"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A19" s="23"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
@@ -7556,12 +7520,12 @@
       <c r="G19" s="15"/>
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
-      <c r="J19" s="63"/>
-      <c r="K19" s="64"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="71"/>
       <c r="L19" s="54"/>
       <c r="M19" s="26"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A20" s="23"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
@@ -7571,12 +7535,12 @@
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
-      <c r="J20" s="63"/>
-      <c r="K20" s="64"/>
+      <c r="J20" s="70"/>
+      <c r="K20" s="71"/>
       <c r="L20" s="54"/>
       <c r="M20" s="26"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A21" s="23"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
@@ -7586,12 +7550,12 @@
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
-      <c r="J21" s="63"/>
-      <c r="K21" s="64"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="71"/>
       <c r="L21" s="54"/>
       <c r="M21" s="26"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A22" s="23"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -7601,12 +7565,12 @@
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
-      <c r="J22" s="63"/>
-      <c r="K22" s="64"/>
+      <c r="J22" s="70"/>
+      <c r="K22" s="71"/>
       <c r="L22" s="54"/>
       <c r="M22" s="26"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A23" s="23"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -7616,12 +7580,12 @@
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
-      <c r="J23" s="63"/>
-      <c r="K23" s="64"/>
+      <c r="J23" s="70"/>
+      <c r="K23" s="71"/>
       <c r="L23" s="54"/>
       <c r="M23" s="26"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A24" s="23"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
@@ -7631,12 +7595,12 @@
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
-      <c r="J24" s="63"/>
-      <c r="K24" s="64"/>
+      <c r="J24" s="70"/>
+      <c r="K24" s="71"/>
       <c r="L24" s="54"/>
       <c r="M24" s="26"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A25" s="23"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
@@ -7646,12 +7610,12 @@
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
       <c r="I25" s="15"/>
-      <c r="J25" s="63"/>
-      <c r="K25" s="64"/>
+      <c r="J25" s="70"/>
+      <c r="K25" s="71"/>
       <c r="L25" s="54"/>
       <c r="M25" s="26"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A26" s="23"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -7661,12 +7625,12 @@
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
       <c r="I26" s="15"/>
-      <c r="J26" s="63"/>
-      <c r="K26" s="64"/>
+      <c r="J26" s="70"/>
+      <c r="K26" s="71"/>
       <c r="L26" s="54"/>
       <c r="M26" s="26"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A27" s="23"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -7676,12 +7640,12 @@
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
-      <c r="J27" s="63"/>
-      <c r="K27" s="64"/>
+      <c r="J27" s="70"/>
+      <c r="K27" s="71"/>
       <c r="L27" s="54"/>
       <c r="M27" s="26"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A28" s="23"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -7691,12 +7655,12 @@
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
-      <c r="J28" s="63"/>
-      <c r="K28" s="64"/>
+      <c r="J28" s="70"/>
+      <c r="K28" s="71"/>
       <c r="L28" s="54"/>
       <c r="M28" s="26"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A29" s="23"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -7706,12 +7670,12 @@
       <c r="G29" s="15"/>
       <c r="H29" s="15"/>
       <c r="I29" s="15"/>
-      <c r="J29" s="63"/>
-      <c r="K29" s="64"/>
+      <c r="J29" s="70"/>
+      <c r="K29" s="71"/>
       <c r="L29" s="54"/>
       <c r="M29" s="26"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A30" s="23"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -7721,12 +7685,12 @@
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
       <c r="I30" s="15"/>
-      <c r="J30" s="63"/>
-      <c r="K30" s="64"/>
+      <c r="J30" s="70"/>
+      <c r="K30" s="71"/>
       <c r="L30" s="54"/>
       <c r="M30" s="26"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A31" s="23"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -7736,12 +7700,12 @@
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
-      <c r="J31" s="63"/>
-      <c r="K31" s="64"/>
+      <c r="J31" s="70"/>
+      <c r="K31" s="71"/>
       <c r="L31" s="54"/>
       <c r="M31" s="26"/>
     </row>
-    <row r="32" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" ht="13.2" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="24"/>
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
@@ -7751,31 +7715,14 @@
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
       <c r="I32" s="19"/>
-      <c r="J32" s="116"/>
-      <c r="K32" s="117"/>
+      <c r="J32" s="124"/>
+      <c r="K32" s="125"/>
       <c r="L32" s="55"/>
       <c r="M32" s="27"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="33">
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J30:K30"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="J32:K32"/>
@@ -7792,43 +7739,43 @@
     <mergeCell ref="J19:K19"/>
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
   </mergeCells>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="expression" dxfId="4" priority="12">
+      <formula>LEN(A6) &gt;30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B13:D32">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>LEN(B13)&gt;30</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="expression" dxfId="7" priority="11">
+    <cfRule type="expression" dxfId="2" priority="11">
       <formula>LEN(F6) &gt;30</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6">
-    <cfRule type="expression" dxfId="6" priority="12">
-      <formula>LEN(A6) &gt;30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13 B17:B32 D13:D32">
-    <cfRule type="expression" dxfId="5" priority="5">
-      <formula>LEN(B13)&gt;30</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I13:I32">
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
+    <cfRule type="expression" dxfId="0" priority="6">
       <formula>LEN(I13)&gt;10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13:I32">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:B16">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>LEN(B14)&gt;30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13 C17:C32">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>LEN(C13)&gt;30</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14:C16">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>LEN(C14)&gt;30</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -7872,7 +7819,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6C9F9DD1-D215-486C-98DE-B297B043F988}">
           <x14:formula1>
-            <xm:f>'Drop Downs'!$F$1:$F$4</xm:f>
+            <xm:f>'Drop Downs'!$F$1:$F$6</xm:f>
           </x14:formula1>
           <xm:sqref>E13:E32</xm:sqref>
         </x14:dataValidation>
@@ -7896,19 +7843,19 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.1796875" customWidth="1"/>
-    <col min="8" max="8" width="18.453125" customWidth="1"/>
-    <col min="9" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7890625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7890625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.15625" customWidth="1"/>
+    <col min="8" max="8" width="18.47265625" customWidth="1"/>
+    <col min="9" max="9" width="9.7890625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.54296875" customWidth="1"/>
+    <col min="13" max="13" width="13.5234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7952,7 +7899,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -7996,7 +7943,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -8034,7 +7981,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -8066,7 +8013,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -8083,7 +8030,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
         <v>48</v>
       </c>
@@ -8097,127 +8044,127 @@
         <v>279</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="G7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="G8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="G9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="G10" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="G11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="G12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="G13" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="G14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="G15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="G16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G22" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G25" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G26" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G27" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G28" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G29" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G30" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G31" t="s">
         <v>38</v>
       </c>
@@ -8236,13 +8183,13 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="28.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>72</v>
       </c>
@@ -8250,7 +8197,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -8258,7 +8205,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -8266,7 +8213,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -8274,7 +8221,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>80</v>
       </c>
@@ -8282,7 +8229,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>82</v>
       </c>
@@ -8290,7 +8237,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -8298,7 +8245,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -8306,7 +8253,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>88</v>
       </c>
@@ -8314,7 +8261,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>90</v>
       </c>
@@ -8322,7 +8269,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>92</v>
       </c>
@@ -8330,7 +8277,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>94</v>
       </c>
@@ -8338,7 +8285,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -8346,7 +8293,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>98</v>
       </c>
@@ -8354,7 +8301,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>100</v>
       </c>
@@ -8362,7 +8309,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>102</v>
       </c>
@@ -8370,7 +8317,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>104</v>
       </c>
@@ -8378,7 +8325,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>106</v>
       </c>
@@ -8386,7 +8333,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>108</v>
       </c>
@@ -8394,7 +8341,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>110</v>
       </c>
@@ -8402,7 +8349,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>112</v>
       </c>
@@ -8410,7 +8357,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -8418,7 +8365,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>113</v>
       </c>
@@ -8426,7 +8373,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>115</v>
       </c>
@@ -8434,7 +8381,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -8442,7 +8389,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>117</v>
       </c>
@@ -8450,7 +8397,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>119</v>
       </c>
@@ -8458,7 +8405,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>121</v>
       </c>
@@ -8466,7 +8413,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>123</v>
       </c>
@@ -8474,7 +8421,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>125</v>
       </c>
@@ -8482,7 +8429,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>127</v>
       </c>
@@ -8490,7 +8437,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>129</v>
       </c>
@@ -8498,7 +8445,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>131</v>
       </c>
@@ -8506,7 +8453,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>133</v>
       </c>
@@ -8514,7 +8461,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>135</v>
       </c>
@@ -8522,7 +8469,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>137</v>
       </c>
@@ -8530,7 +8477,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>139</v>
       </c>
@@ -8538,7 +8485,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>141</v>
       </c>
@@ -8546,7 +8493,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>143</v>
       </c>
@@ -8554,7 +8501,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>145</v>
       </c>
@@ -8562,7 +8509,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>147</v>
       </c>
@@ -8570,7 +8517,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>149</v>
       </c>
@@ -8578,7 +8525,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>151</v>
       </c>
@@ -8586,7 +8533,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>153</v>
       </c>
@@ -8594,7 +8541,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>155</v>
       </c>
@@ -8602,7 +8549,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>157</v>
       </c>
@@ -8610,7 +8557,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>159</v>
       </c>
@@ -8618,7 +8565,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>161</v>
       </c>
@@ -8626,7 +8573,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>163</v>
       </c>
@@ -8634,7 +8581,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>165</v>
       </c>
@@ -8642,7 +8589,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>167</v>
       </c>
@@ -8650,7 +8597,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>169</v>
       </c>
@@ -8658,7 +8605,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>171</v>
       </c>
@@ -8666,7 +8613,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>173</v>
       </c>
@@ -8674,7 +8621,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -8682,7 +8629,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>175</v>
       </c>
@@ -8690,7 +8637,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
         <v>177</v>
       </c>
@@ -8698,7 +8645,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>179</v>
       </c>
@@ -8706,7 +8653,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>181</v>
       </c>
@@ -8714,7 +8661,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>183</v>
       </c>
@@ -8722,7 +8669,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>185</v>
       </c>
@@ -8730,7 +8677,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>187</v>
       </c>
@@ -8738,7 +8685,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
         <v>189</v>
       </c>
@@ -8746,7 +8693,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>191</v>
       </c>
@@ -8754,7 +8701,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>193</v>
       </c>
@@ -8762,7 +8709,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>195</v>
       </c>
@@ -8770,7 +8717,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>197</v>
       </c>
@@ -8778,7 +8725,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>199</v>
       </c>
@@ -8786,7 +8733,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
         <v>201</v>
       </c>
@@ -8794,7 +8741,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>203</v>
       </c>
@@ -8802,7 +8749,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>205</v>
       </c>
@@ -8810,7 +8757,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>207</v>
       </c>
@@ -8818,7 +8765,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
         <v>209</v>
       </c>
@@ -8826,7 +8773,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
         <v>211</v>
       </c>
@@ -8834,7 +8781,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
         <v>213</v>
       </c>
@@ -8842,7 +8789,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>215</v>
       </c>
@@ -8850,7 +8797,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
         <v>217</v>
       </c>
@@ -8858,7 +8805,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
         <v>219</v>
       </c>
@@ -8866,7 +8813,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
         <v>221</v>
       </c>
@@ -8874,7 +8821,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
         <v>223</v>
       </c>
@@ -8882,7 +8829,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
         <v>225</v>
       </c>
@@ -8899,21 +8846,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DED4A2CA298C634D861C291708FBD60B" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e9dad94b1987da259c39e2ef3e1e6b7a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -9027,34 +8963,30 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{659DA32C-5651-4ED5-961A-CEDF94F65B02}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF3B6C40-1D0B-4E20-A005-7908467DF3DF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA75E35D-C619-45E2-A921-889D8A13153B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F3BCE80-3643-4525-B9BB-BDD667043D24}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9070,10 +9002,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA75E35D-C619-45E2-A921-889D8A13153B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF3B6C40-1D0B-4E20-A005-7908467DF3DF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{659DA32C-5651-4ED5-961A-CEDF94F65B02}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>